<commit_message>
modificaciones de reporte diario
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/FisProductos.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/FisProductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320ED208-2A61-4BB2-8B14-A9347A46D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E40EC9-C7BC-4F6A-8FB3-962EF1D6B2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1A8A820-0DC8-4494-B741-8ACF5A2C6F65}"/>
   </bookViews>
@@ -139,55 +139,55 @@
     <t>Observaciones</t>
   </si>
   <si>
+    <t>___________________</t>
+  </si>
+  <si>
+    <t>GLP</t>
+  </si>
+  <si>
+    <t>CGN</t>
+  </si>
+  <si>
+    <t>{{GlpProduccion}}</t>
+  </si>
+  <si>
+    <t>{{CgnProduccion}}</t>
+  </si>
+  <si>
+    <t>{{CgnInventario}}</t>
+  </si>
+  <si>
+    <t>{{CgnDespacho}}</t>
+  </si>
+  <si>
+    <t>{{GlpDespacho}}</t>
+  </si>
+  <si>
+    <t>{{GlpInventario}}</t>
+  </si>
+  <si>
+    <t>{{TotalProduccion}}</t>
+  </si>
+  <si>
+    <t>{{TotalDespacho}}</t>
+  </si>
+  <si>
+    <t>{{TotalInventario}}</t>
+  </si>
+  <si>
+    <t>{{TotalGlpInventario}}</t>
+  </si>
+  <si>
+    <t>{{TotalGlpNivel}}</t>
+  </si>
+  <si>
+    <t>{{TotalCgnNivel}}</t>
+  </si>
+  <si>
+    <t>{{TotalCgnInventario}}</t>
+  </si>
+  <si>
     <t>________________</t>
-  </si>
-  <si>
-    <t>___________________</t>
-  </si>
-  <si>
-    <t>GLP</t>
-  </si>
-  <si>
-    <t>CGN</t>
-  </si>
-  <si>
-    <t>{{GlpProduccion}}</t>
-  </si>
-  <si>
-    <t>{{CgnProduccion}}</t>
-  </si>
-  <si>
-    <t>{{CgnInventario}}</t>
-  </si>
-  <si>
-    <t>{{CgnDespacho}}</t>
-  </si>
-  <si>
-    <t>{{GlpDespacho}}</t>
-  </si>
-  <si>
-    <t>{{GlpInventario}}</t>
-  </si>
-  <si>
-    <t>{{TotalProduccion}}</t>
-  </si>
-  <si>
-    <t>{{TotalDespacho}}</t>
-  </si>
-  <si>
-    <t>{{TotalInventario}}</t>
-  </si>
-  <si>
-    <t>{{TotalGlpInventario}}</t>
-  </si>
-  <si>
-    <t>{{TotalGlpNivel}}</t>
-  </si>
-  <si>
-    <t>{{TotalCgnNivel}}</t>
-  </si>
-  <si>
-    <t>{{TotalCgnInventario}}</t>
   </si>
 </sst>
 </file>
@@ -527,9 +527,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -550,9 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,6 +647,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -662,53 +704,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,56 +784,6 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>36636</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>14653</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>996839</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>129012</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC85540-0589-4839-AD8C-9DB6927C5394}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1282213" y="5942134"/>
-          <a:ext cx="960203" cy="685859"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1140,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849CC9BB-3F6A-4ED2-8708-37259B7D1880}">
   <dimension ref="A1:XFB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15"/>
@@ -1159,82 +1109,82 @@
   <sheetData>
     <row r="1" spans="1:7" ht="12" customHeight="1">
       <c r="A1" s="72"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="62" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="63"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7" ht="12" customHeight="1">
       <c r="A2" s="72"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="65" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="66"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:7" ht="12" customHeight="1">
       <c r="A3" s="72"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="67" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="68"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" ht="12" customHeight="1">
       <c r="A4" s="72"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="18" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12" customHeight="1">
       <c r="A5" s="72"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="20" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
     </row>
     <row r="8" spans="1:7" ht="9.9499999999999993" customHeight="1"/>
     <row r="9" spans="1:7">
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="35" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="2"/>
@@ -1247,10 +1197,10 @@
       <c r="C11" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="10"/>
@@ -1258,10 +1208,10 @@
     <row r="12" spans="1:7" ht="12.95" customHeight="1">
       <c r="B12" s="74"/>
       <c r="C12" s="74"/>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="38" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="10"/>
@@ -1270,10 +1220,10 @@
       <c r="B13" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="78" t="s">
+      <c r="D13" s="62" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1283,10 +1233,10 @@
     </row>
     <row r="14" spans="1:7" ht="12.95" customHeight="1">
       <c r="B14" s="75"/>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="79" t="s">
+      <c r="D14" s="63" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -1296,20 +1246,20 @@
     </row>
     <row r="15" spans="1:7" ht="12.95" customHeight="1">
       <c r="B15" s="75"/>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="41" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:7" ht="12.95" customHeight="1">
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
     </row>
     <row r="17" spans="2:6" ht="12.95" customHeight="1">
       <c r="B17" s="73" t="s">
@@ -1318,64 +1268,64 @@
       <c r="C17" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="37" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="12.95" customHeight="1">
       <c r="B18" s="74"/>
       <c r="C18" s="74"/>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="38" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="46" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B20" s="59"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B21" s="54"/>
-      <c r="C21" s="55" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="55" t="s">
+      <c r="D21" s="54" t="s">
         <v>49</v>
       </c>
+      <c r="E21" s="53" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
     </row>
     <row r="23" spans="2:6" ht="12.95" customHeight="1">
       <c r="B23" s="73" t="s">
@@ -1384,10 +1334,10 @@
       <c r="C23" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="9"/>
@@ -1395,134 +1345,134 @@
     <row r="24" spans="2:6" ht="12.95" customHeight="1">
       <c r="B24" s="74"/>
       <c r="C24" s="74"/>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="38" t="s">
         <v>30</v>
       </c>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="51" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B26" s="61"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B27" s="58"/>
-      <c r="C27" s="55" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="56" t="s">
+      <c r="D27" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="55" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="28" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="2:6" ht="12.95" customHeight="1">
       <c r="B29" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F29" s="10"/>
     </row>
     <row r="30" spans="2:6" ht="12.95" customHeight="1">
       <c r="B30" s="74"/>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="38" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" spans="2:6" ht="12.95" customHeight="1">
+      <c r="B32" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C32" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="32" t="s">
+      <c r="D32" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="2:6" ht="12.95" customHeight="1">
+      <c r="B33" s="25"/>
+      <c r="C33" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B32" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="26"/>
-    </row>
-    <row r="33" spans="2:6" ht="12.95" customHeight="1">
-      <c r="B33" s="27"/>
-      <c r="C33" s="28" t="s">
+      <c r="D33" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="E33" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="3"/>
-      <c r="C34" s="25"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="1"/>
@@ -1531,58 +1481,57 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="16"/>
+      <c r="B39" s="79"/>
     </row>
     <row r="40" spans="2:6">
-      <c r="B40" s="16"/>
+      <c r="B40" s="79"/>
     </row>
     <row r="41" spans="2:6">
-      <c r="B41" s="16"/>
+      <c r="B41" s="79"/>
     </row>
     <row r="42" spans="2:6">
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="70"/>
+      <c r="E42" s="69"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="69" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="69"/>
-      <c r="F43" s="23"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C11:C12"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B36:E38"/>
     <mergeCell ref="F2:G2"/>
@@ -1599,6 +1548,7 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>